<commit_message>
add second order similarity
</commit_message>
<xml_diff>
--- a/blog/22_1_22_24_chord_similarity/chord_vectors.xlsx
+++ b/blog/22_1_22_24_chord_similarity/chord_vectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattcrump/Github/homophony.github.io/blog/22_1_22_24_chord_similarity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4F964B0-6A9E-C44B-8C2E-C01A7D9C08A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7883C6F-FBFA-834F-AB68-2432C7E09539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="500" windowWidth="12840" windowHeight="25060" xr2:uid="{8745B402-A4AF-EE43-9072-997B8CB9258E}"/>
+    <workbookView xWindow="2280" yWindow="500" windowWidth="25920" windowHeight="23100" xr2:uid="{8745B402-A4AF-EE43-9072-997B8CB9258E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>C</t>
   </si>
@@ -158,6 +158,9 @@
     <t>Cm11(b5)</t>
   </si>
   <si>
+    <t>sus</t>
+  </si>
+  <si>
     <t>Csus</t>
   </si>
   <si>
@@ -213,6 +216,36 @@
   </si>
   <si>
     <t>C7#11#9</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>scale</t>
+  </si>
+  <si>
+    <t>triads</t>
+  </si>
+  <si>
+    <t>dominant 7th</t>
+  </si>
+  <si>
+    <t>major 7th</t>
+  </si>
+  <si>
+    <t>minor 7th</t>
+  </si>
+  <si>
+    <t>half-diminished 7th</t>
+  </si>
+  <si>
+    <t>altered</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -584,71 +617,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE852C40-E600-314E-B909-74AEA2B2C84C}">
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+      <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="13" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="15" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -677,17 +716,23 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
@@ -698,10 +743,10 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -718,40 +763,46 @@
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -759,40 +810,46 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -800,34 +857,40 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -839,36 +902,42 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -880,19 +949,25 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
       <c r="D8">
         <v>1</v>
       </c>
@@ -906,16 +981,16 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -923,40 +998,46 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -964,58 +1045,70 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11">
         <v>1</v>
       </c>
@@ -1029,34 +1122,40 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -1073,31 +1172,37 @@
         <v>1</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
       <c r="D13">
         <v>1</v>
       </c>
@@ -1111,10 +1216,10 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1123,22 +1228,28 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="D14">
         <v>1</v>
       </c>
@@ -1155,72 +1266,84 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
         <v>26</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
       <c r="D16">
         <v>1</v>
       </c>
@@ -1234,34 +1357,40 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
         <v>27</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
       <c r="D17">
         <v>1</v>
       </c>
@@ -1278,31 +1407,37 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
         <v>28</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
       <c r="D18">
         <v>1</v>
       </c>
@@ -1319,10 +1454,10 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1333,66 +1468,78 @@
       <c r="M18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1404,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1413,109 +1560,127 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
         <v>32</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1530,30 +1695,36 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1571,33 +1742,39 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
         <v>35</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1615,188 +1792,218 @@
         <v>1</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
         <v>37</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>0</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>39</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
         <v>40</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
+      <c r="C30" t="s">
+        <v>41</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1805,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1817,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1825,19 +2032,25 @@
       <c r="M30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1846,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -1858,24 +2071,30 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1884,10 +2103,10 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -1899,24 +2118,30 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1925,10 +2150,10 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1943,33 +2168,39 @@
         <v>1</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -1981,36 +2212,42 @@
         <v>0</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>46</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -2025,30 +2262,36 @@
         <v>1</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>47</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2060,48 +2303,54 @@
         <v>0</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>48</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -2112,69 +2361,81 @@
       <c r="M37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -2183,48 +2444,54 @@
         <v>0</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <v>0</v>
       </c>
       <c r="J40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -2235,25 +2502,31 @@
       <c r="M40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2265,48 +2538,54 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
       <c r="L41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>53</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <v>0</v>
       </c>
       <c r="J42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -2317,119 +2596,137 @@
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43">
         <v>0</v>
       </c>
       <c r="M43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" t="s">
+        <v>55</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
       <c r="K44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
       <c r="M44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" t="s">
+        <v>56</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45">
         <v>0</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <v>0</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -2440,78 +2737,90 @@
       <c r="M45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46">
         <v>0</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46">
         <v>0</v>
       </c>
       <c r="M46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -2520,47 +2829,59 @@
         <v>0</v>
       </c>
       <c r="M47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48">
         <v>0</v>
       </c>
     </row>

</xml_diff>